<commit_message>
Revert "Fixed if statement"
This reverts commit 60ff70f629240c8ff994efd121d33452464f937e.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>fluxes</t>
   </si>
@@ -530,9 +530,6 @@
   </si>
   <si>
     <t>Succinate_import</t>
-  </si>
-  <si>
-    <t>Succinate_export</t>
   </si>
   <si>
     <t>H_import</t>
@@ -1106,7 +1103,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B245"/>
+  <dimension ref="A1:B244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2490,7 +2487,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>0</v>
+        <v>2.119437399123813</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2498,7 +2495,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>2.119437399123813</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2602,7 +2599,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>0</v>
+        <v>3.414341710860045</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2610,7 +2607,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>3.414341710860045</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2634,7 +2631,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>0</v>
+        <v>-4.980401198985474</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2642,7 +2639,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>-4.980401198985474</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2666,7 +2663,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>0</v>
+        <v>-2.414111136730463</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2674,7 +2671,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>-2.414111136730463</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2682,7 +2679,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>0</v>
+        <v>-1.727922527092457</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2690,7 +2687,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>-1.727922527092457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2698,7 +2695,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>0</v>
+        <v>-0.3956652063638459</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2706,7 +2703,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>-0.3956652063638459</v>
+        <v>1.566059488125429</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2714,7 +2711,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>1.566059488125429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2762,7 +2759,7 @@
         <v>206</v>
       </c>
       <c r="B207">
-        <v>0</v>
+        <v>-0.4233341019137651</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2770,7 +2767,7 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>-0.4233341019137651</v>
+        <v>-1.228745796218758e-16</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2778,7 +2775,7 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>-1.228745796218758e-16</v>
+        <v>0.8010145261701633</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2786,7 +2783,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0.8010145261701633</v>
+        <v>-2.57597417569749</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2794,7 +2791,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>-2.57597417569749</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2802,7 +2799,7 @@
         <v>211</v>
       </c>
       <c r="B212">
-        <v>0</v>
+        <v>-2.546921835370068</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2810,7 +2807,7 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>-2.546921835370068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2818,7 +2815,7 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>0</v>
+        <v>1.228745796218758e-16</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2826,7 +2823,7 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>1.228745796218758e-16</v>
+        <v>-1.110223024625156e-16</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2834,7 +2831,7 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>-1.110223024625156e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2874,7 +2871,7 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>0</v>
+        <v>2.546921835370068</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2882,7 +2879,7 @@
         <v>221</v>
       </c>
       <c r="B222">
-        <v>2.546921835370068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2906,7 +2903,7 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>0</v>
+        <v>0.06778879409730348</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2938,7 +2935,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>0.06778879409730348</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2970,7 +2967,7 @@
         <v>232</v>
       </c>
       <c r="B233">
-        <v>0</v>
+        <v>-0.04011989854738298</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2994,7 +2991,7 @@
         <v>235</v>
       </c>
       <c r="B236">
-        <v>-0.04011989854738298</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -3058,14 +3055,6 @@
         <v>243</v>
       </c>
       <c r="B244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2">
-      <c r="A245" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B245">
         <v>-1.110223024625157e-16</v>
       </c>
     </row>

</xml_diff>